<commit_message>
add can afford to build check
</commit_message>
<xml_diff>
--- a/CityBuilder/resources/configEditor.xlsx
+++ b/CityBuilder/resources/configEditor.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3255" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3255"/>
   </bookViews>
   <sheets>
     <sheet name="editable" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>This row intentionally left blank.</t>
   </si>
@@ -72,9 +72,6 @@
     <t>menu_order</t>
   </si>
   <si>
-    <t>reasource_req</t>
-  </si>
-  <si>
     <t>produces</t>
   </si>
   <si>
@@ -94,6 +91,12 @@
   </si>
   <si>
     <t>{"x":0, "y":-10}</t>
+  </si>
+  <si>
+    <t>resource_req</t>
+  </si>
+  <si>
+    <t>{}</t>
   </si>
 </sst>
 </file>
@@ -456,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,10 +494,10 @@
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -513,8 +516,11 @@
       <c r="E2" t="s">
         <v>1</v>
       </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -534,13 +540,13 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
         <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -560,10 +566,10 @@
         <v>12</v>
       </c>
       <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
         <v>19</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -576,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="A2:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +620,7 @@
       </c>
       <c r="G2" t="str">
         <f>IF(LEN(editable!G2)&gt;0,_xlfn.CONCAT(editable!G$1,"=",editable!G2),"")</f>
-        <v/>
+        <v>resource_req={}</v>
       </c>
       <c r="H2" t="str">
         <f>IF(LEN(editable!H2)&gt;0,_xlfn.CONCAT(editable!H$1,"=",editable!H2),"")</f>
@@ -688,7 +694,7 @@
       </c>
       <c r="G3" t="str">
         <f>IF(LEN(editable!G3)&gt;0,_xlfn.CONCAT(editable!G$1,"=",editable!G3),"")</f>
-        <v>reasource_req={"pop": 3}</v>
+        <v>resource_req={"pop": 3}</v>
       </c>
       <c r="H3" t="str">
         <f>IF(LEN(editable!H3)&gt;0,_xlfn.CONCAT(editable!H$1,"=",editable!H3),"")</f>
@@ -762,7 +768,7 @@
       </c>
       <c r="G4" t="str">
         <f>IF(LEN(editable!G4)&gt;0,_xlfn.CONCAT(editable!G$1,"=",editable!G4),"")</f>
-        <v>reasource_req={"food": 3}</v>
+        <v>resource_req={"food": 3}</v>
       </c>
       <c r="H4" t="str">
         <f>IF(LEN(editable!H4)&gt;0,_xlfn.CONCAT(editable!H$1,"=",editable!H4),"")</f>

</xml_diff>

<commit_message>
Added water and shore
Mostly image updates
</commit_message>
<xml_diff>
--- a/CityBuilder/resources/configEditor.xlsx
+++ b/CityBuilder/resources/configEditor.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keziah\Documents\GoDot\CityBuilder\godotCityBuilder\CityBuilder\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Slaughter\Documents\GitHub\godotCityBuilder\CityBuilder\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3255" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3255" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="editable" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="123">
   <si>
     <t>This row intentionally left blank.</t>
   </si>
@@ -391,12 +391,15 @@
   </si>
   <si>
     <t>"Reservoir"</t>
+  </si>
+  <si>
+    <t>["shore"]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -753,11 +756,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1187,7 +1190,7 @@
         <v>17</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>46</v>
@@ -2100,7 +2103,7 @@
         <v>17</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>63</v>
@@ -2366,10 +2369,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:K45"/>
     </sheetView>
   </sheetViews>
@@ -3079,7 +3082,7 @@
       </c>
       <c r="G12" t="str">
         <f>IF(LEN(editable!I12)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I12),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["shore"]</v>
       </c>
       <c r="H12" t="str">
         <f>IF(LEN(editable!J12)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J12),"")</f>
@@ -4591,7 +4594,7 @@
       </c>
       <c r="G38" t="str">
         <f>IF(LEN(editable!I38)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I38),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["shore"]</v>
       </c>
       <c r="H38" t="str">
         <f>IF(LEN(editable!J38)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J38),"")</f>

</xml_diff>

<commit_message>
large buildings test build conditions properlt
</commit_message>
<xml_diff>
--- a/CityBuilder/resources/configEditor.xlsx
+++ b/CityBuilder/resources/configEditor.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Slaughter\Documents\GitHub\godotCityBuilder\CityBuilder\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keziah\Documents\GoDot\CityBuilder\godotCityBuilder\CityBuilder\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3255" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3255" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="editable" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>buildable_tiles</t>
   </si>
   <si>
-    <t>["grass", "farmland"]</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -394,12 +391,15 @@
   </si>
   <si>
     <t>["shore"]</t>
+  </si>
+  <si>
+    <t>["grass", "farmland", "shore"]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -756,11 +756,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView topLeftCell="C28" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,28 +778,28 @@
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>3</v>
@@ -808,24 +808,24 @@
         <v>1</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -834,33 +834,33 @@
         <v>10</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" s="3">
         <v>2</v>
@@ -869,33 +869,33 @@
         <v>10</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" s="3">
         <v>3</v>
@@ -904,33 +904,33 @@
         <v>10</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" s="3">
         <v>4</v>
@@ -939,33 +939,33 @@
         <v>10</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E6" s="3">
         <v>5</v>
@@ -974,33 +974,33 @@
         <v>10</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E7" s="3">
         <v>6</v>
@@ -1009,33 +1009,33 @@
         <v>10</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E8" s="3">
         <v>7</v>
@@ -1044,33 +1044,33 @@
         <v>10</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E9" s="3">
         <v>8</v>
@@ -1079,33 +1079,33 @@
         <v>10</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E10" s="3">
         <v>9</v>
@@ -1114,33 +1114,33 @@
         <v>10</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E11" s="3">
         <v>10</v>
@@ -1149,33 +1149,33 @@
         <v>10</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="3">
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E12" s="3">
         <v>11</v>
@@ -1184,33 +1184,33 @@
         <v>100</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="3">
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E13" s="3">
         <v>12</v>
@@ -1219,33 +1219,33 @@
         <v>100</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="3">
         <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E14" s="3">
         <v>13</v>
@@ -1254,33 +1254,33 @@
         <v>100</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="3">
         <v>2</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E15" s="3">
         <v>14</v>
@@ -1289,33 +1289,33 @@
         <v>100</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="3">
         <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E16" s="3">
         <v>15</v>
@@ -1324,33 +1324,33 @@
         <v>100</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="3">
         <v>2</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E17" s="3">
         <v>16</v>
@@ -1359,33 +1359,33 @@
         <v>100</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="3">
         <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E18" s="3">
         <v>17</v>
@@ -1394,36 +1394,36 @@
         <v>100</v>
       </c>
       <c r="G18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="I18" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="3">
         <v>2</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E19" s="3">
         <v>18</v>
@@ -1432,33 +1432,33 @@
         <v>100</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="3">
         <v>2</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E20" s="3">
         <v>19</v>
@@ -1467,33 +1467,33 @@
         <v>100</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="3">
         <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E21" s="3">
         <v>20</v>
@@ -1502,33 +1502,33 @@
         <v>100</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="3">
         <v>2</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E22" s="3">
         <v>21</v>
@@ -1537,33 +1537,33 @@
         <v>100</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" s="3">
         <v>2</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E23" s="3">
         <v>22</v>
@@ -1572,33 +1572,33 @@
         <v>100</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" s="3">
         <v>2</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E24" s="3">
         <v>23</v>
@@ -1607,33 +1607,33 @@
         <v>100</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="3">
         <v>2</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E25" s="3">
         <v>24</v>
@@ -1642,33 +1642,33 @@
         <v>100</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C26" s="3">
         <v>2</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E26" s="3">
         <v>25</v>
@@ -1677,33 +1677,33 @@
         <v>100</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="3">
         <v>2</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E27" s="3">
         <v>26</v>
@@ -1712,33 +1712,33 @@
         <v>100</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28" s="3">
         <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E28" s="3">
         <v>27</v>
@@ -1747,33 +1747,33 @@
         <v>100</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C29" s="2">
         <v>2</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E29" s="3">
         <v>28</v>
@@ -1782,33 +1782,33 @@
         <v>100</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C30" s="3">
         <v>3</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E30" s="3">
         <v>29</v>
@@ -1817,33 +1817,33 @@
         <v>1000</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C31" s="3">
         <v>3</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E31" s="3">
         <v>30</v>
@@ -1852,33 +1852,33 @@
         <v>1000</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C32" s="3">
         <v>3</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E32" s="3">
         <v>31</v>
@@ -1887,33 +1887,33 @@
         <v>1000</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C33" s="3">
         <v>3</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E33" s="3">
         <v>32</v>
@@ -1922,33 +1922,33 @@
         <v>1000</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C34" s="3">
         <v>3</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E34" s="3">
         <v>33</v>
@@ -1957,33 +1957,33 @@
         <v>1000</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C35" s="3">
         <v>3</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E35" s="3">
         <v>34</v>
@@ -1992,33 +1992,33 @@
         <v>1000</v>
       </c>
       <c r="G35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H35" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="I35" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C36" s="3">
         <v>3</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E36" s="3">
         <v>35</v>
@@ -2027,33 +2027,33 @@
         <v>1000</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C37" s="3">
         <v>3</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E37" s="3">
         <v>36</v>
@@ -2062,33 +2062,33 @@
         <v>1000</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C38" s="3">
         <v>3</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E38" s="3">
         <v>37</v>
@@ -2097,33 +2097,33 @@
         <v>1000</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C39" s="3">
         <v>3</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E39" s="3">
         <v>38</v>
@@ -2132,33 +2132,33 @@
         <v>1000</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C40" s="3">
         <v>3</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E40" s="3">
         <v>39</v>
@@ -2167,33 +2167,33 @@
         <v>1000</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C41" s="3">
         <v>3</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E41" s="3">
         <v>40</v>
@@ -2202,33 +2202,33 @@
         <v>1000</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C42" s="3">
         <v>3</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E42" s="3">
         <v>41</v>
@@ -2237,33 +2237,33 @@
         <v>1000</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C43" s="3">
         <v>3</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E43" s="3">
         <v>42</v>
@@ -2272,33 +2272,33 @@
         <v>1000</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C44" s="3">
         <v>3</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E44" s="3">
         <v>43</v>
@@ -2307,33 +2307,33 @@
         <v>1000</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C45" s="2">
         <v>3</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E45" s="3">
         <v>44</v>
@@ -2342,19 +2342,19 @@
         <v>1000</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2369,10 +2369,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:K45"/>
     </sheetView>
   </sheetViews>
@@ -2492,7 +2492,7 @@
       </c>
       <c r="G3" t="str">
         <f>IF(LEN(editable!I3)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I3),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H3" t="str">
         <f>IF(LEN(editable!J3)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J3),"")</f>
@@ -2570,7 +2570,7 @@
       </c>
       <c r="G4" t="str">
         <f>IF(LEN(editable!I4)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I4),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H4" t="str">
         <f>IF(LEN(editable!J4)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J4),"")</f>
@@ -2648,7 +2648,7 @@
       </c>
       <c r="G5" t="str">
         <f>IF(LEN(editable!I5)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I5),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H5" t="str">
         <f>IF(LEN(editable!J5)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J5),"")</f>
@@ -2710,7 +2710,7 @@
       </c>
       <c r="G6" t="str">
         <f>IF(LEN(editable!I6)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I6),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H6" t="str">
         <f>IF(LEN(editable!J6)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J6),"")</f>
@@ -2772,7 +2772,7 @@
       </c>
       <c r="G7" t="str">
         <f>IF(LEN(editable!I7)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I7),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H7" t="str">
         <f>IF(LEN(editable!J7)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J7),"")</f>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="G8" t="str">
         <f>IF(LEN(editable!I8)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I8),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H8" t="str">
         <f>IF(LEN(editable!J8)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J8),"")</f>
@@ -2896,7 +2896,7 @@
       </c>
       <c r="G9" t="str">
         <f>IF(LEN(editable!I9)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I9),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H9" t="str">
         <f>IF(LEN(editable!J9)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J9),"")</f>
@@ -2958,7 +2958,7 @@
       </c>
       <c r="G10" t="str">
         <f>IF(LEN(editable!I10)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I10),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H10" t="str">
         <f>IF(LEN(editable!J10)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J10),"")</f>
@@ -3020,7 +3020,7 @@
       </c>
       <c r="G11" t="str">
         <f>IF(LEN(editable!I11)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I11),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H11" t="str">
         <f>IF(LEN(editable!J11)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J11),"")</f>
@@ -3202,7 +3202,7 @@
       </c>
       <c r="G14" t="str">
         <f>IF(LEN(editable!I14)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I14),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H14" t="str">
         <f>IF(LEN(editable!J14)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J14),"")</f>
@@ -3260,7 +3260,7 @@
       </c>
       <c r="G15" t="str">
         <f>IF(LEN(editable!I15)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I15),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H15" t="str">
         <f>IF(LEN(editable!J15)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J15),"")</f>
@@ -3318,7 +3318,7 @@
       </c>
       <c r="G16" t="str">
         <f>IF(LEN(editable!I16)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I16),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H16" t="str">
         <f>IF(LEN(editable!J16)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J16),"")</f>
@@ -3376,7 +3376,7 @@
       </c>
       <c r="G17" t="str">
         <f>IF(LEN(editable!I17)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I17),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H17" t="str">
         <f>IF(LEN(editable!J17)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J17),"")</f>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="G18" t="str">
         <f>IF(LEN(editable!I18)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I18),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H18" t="str">
         <f>IF(LEN(editable!J18)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J18),"")</f>
@@ -3492,7 +3492,7 @@
       </c>
       <c r="G19" t="str">
         <f>IF(LEN(editable!I19)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I19),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H19" t="str">
         <f>IF(LEN(editable!J19)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J19),"")</f>
@@ -3550,7 +3550,7 @@
       </c>
       <c r="G20" t="str">
         <f>IF(LEN(editable!I20)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I20),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H20" t="str">
         <f>IF(LEN(editable!J20)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J20),"")</f>
@@ -3608,7 +3608,7 @@
       </c>
       <c r="G21" t="str">
         <f>IF(LEN(editable!I21)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I21),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H21" t="str">
         <f>IF(LEN(editable!J21)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J21),"")</f>
@@ -3666,7 +3666,7 @@
       </c>
       <c r="G22" t="str">
         <f>IF(LEN(editable!I22)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I22),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H22" t="str">
         <f>IF(LEN(editable!J22)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J22),"")</f>
@@ -3724,7 +3724,7 @@
       </c>
       <c r="G23" t="str">
         <f>IF(LEN(editable!I23)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I23),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H23" t="str">
         <f>IF(LEN(editable!J23)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J23),"")</f>
@@ -3782,7 +3782,7 @@
       </c>
       <c r="G24" t="str">
         <f>IF(LEN(editable!I24)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I24),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H24" t="str">
         <f>IF(LEN(editable!J24)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J24),"")</f>
@@ -3840,7 +3840,7 @@
       </c>
       <c r="G25" t="str">
         <f>IF(LEN(editable!I25)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I25),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H25" t="str">
         <f>IF(LEN(editable!J25)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J25),"")</f>
@@ -3898,7 +3898,7 @@
       </c>
       <c r="G26" t="str">
         <f>IF(LEN(editable!I26)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I26),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H26" t="str">
         <f>IF(LEN(editable!J26)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J26),"")</f>
@@ -3956,7 +3956,7 @@
       </c>
       <c r="G27" t="str">
         <f>IF(LEN(editable!I27)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I27),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H27" t="str">
         <f>IF(LEN(editable!J27)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J27),"")</f>
@@ -4014,7 +4014,7 @@
       </c>
       <c r="G28" t="str">
         <f>IF(LEN(editable!I28)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I28),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H28" t="str">
         <f>IF(LEN(editable!J28)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J28),"")</f>
@@ -4072,7 +4072,7 @@
       </c>
       <c r="G29" t="str">
         <f>IF(LEN(editable!I29)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I29),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H29" t="str">
         <f>IF(LEN(editable!J29)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J29),"")</f>
@@ -4130,7 +4130,7 @@
       </c>
       <c r="G30" t="str">
         <f>IF(LEN(editable!I30)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I30),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H30" t="str">
         <f>IF(LEN(editable!J30)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J30),"")</f>
@@ -4188,7 +4188,7 @@
       </c>
       <c r="G31" t="str">
         <f>IF(LEN(editable!I31)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I31),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H31" t="str">
         <f>IF(LEN(editable!J31)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J31),"")</f>
@@ -4246,7 +4246,7 @@
       </c>
       <c r="G32" t="str">
         <f>IF(LEN(editable!I32)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I32),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H32" t="str">
         <f>IF(LEN(editable!J32)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J32),"")</f>
@@ -4304,7 +4304,7 @@
       </c>
       <c r="G33" t="str">
         <f>IF(LEN(editable!I33)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I33),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H33" t="str">
         <f>IF(LEN(editable!J33)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J33),"")</f>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="G34" t="str">
         <f>IF(LEN(editable!I34)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I34),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H34" t="str">
         <f>IF(LEN(editable!J34)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J34),"")</f>
@@ -4420,7 +4420,7 @@
       </c>
       <c r="G35" t="str">
         <f>IF(LEN(editable!I35)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I35),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H35" t="str">
         <f>IF(LEN(editable!J35)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J35),"")</f>
@@ -4478,7 +4478,7 @@
       </c>
       <c r="G36" t="str">
         <f>IF(LEN(editable!I36)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I36),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H36" t="str">
         <f>IF(LEN(editable!J36)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J36),"")</f>
@@ -4536,7 +4536,7 @@
       </c>
       <c r="G37" t="str">
         <f>IF(LEN(editable!I37)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I37),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H37" t="str">
         <f>IF(LEN(editable!J37)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J37),"")</f>
@@ -4652,7 +4652,7 @@
       </c>
       <c r="G39" t="str">
         <f>IF(LEN(editable!I39)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I39),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H39" t="str">
         <f>IF(LEN(editable!J39)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J39),"")</f>
@@ -4710,7 +4710,7 @@
       </c>
       <c r="G40" t="str">
         <f>IF(LEN(editable!I40)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I40),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H40" t="str">
         <f>IF(LEN(editable!J40)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J40),"")</f>
@@ -4768,7 +4768,7 @@
       </c>
       <c r="G41" t="str">
         <f>IF(LEN(editable!I41)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I41),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H41" t="str">
         <f>IF(LEN(editable!J41)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J41),"")</f>
@@ -4826,7 +4826,7 @@
       </c>
       <c r="G42" t="str">
         <f>IF(LEN(editable!I42)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I42),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H42" t="str">
         <f>IF(LEN(editable!J42)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J42),"")</f>
@@ -4884,7 +4884,7 @@
       </c>
       <c r="G43" t="str">
         <f>IF(LEN(editable!I43)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I43),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H43" t="str">
         <f>IF(LEN(editable!J43)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J43),"")</f>
@@ -4942,7 +4942,7 @@
       </c>
       <c r="G44" t="str">
         <f>IF(LEN(editable!I44)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I44),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H44" t="str">
         <f>IF(LEN(editable!J44)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J44),"")</f>
@@ -5000,7 +5000,7 @@
       </c>
       <c r="G45" t="str">
         <f>IF(LEN(editable!I45)&gt;0,_xlfn.CONCAT(editable!I$1,"=",editable!I45),"")</f>
-        <v>buildable_tiles=["grass", "farmland"]</v>
+        <v>buildable_tiles=["grass", "farmland", "shore"]</v>
       </c>
       <c r="H45" t="str">
         <f>IF(LEN(editable!J45)&gt;0,_xlfn.CONCAT(editable!J$1,"=",editable!J45),"")</f>

</xml_diff>